<commit_message>
split methods by part
</commit_message>
<xml_diff>
--- a/Iteration4/time_log.xlsx
+++ b/Iteration4/time_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdw12_000\Desktop\Ara\BCPR280_Part1\Iteration4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86BF93B-CD91-45E3-ACFB-4DD532BA3E6C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D10C12-0E9E-49E2-8C37-A217CAE4C46F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1560" windowWidth="16755" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1019,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1141,29 +1141,29 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C12" s="14">
         <v>43568</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="H10" t="s">
+      <c r="D12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="H12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C13" s="14">
         <v>43568</v>
       </c>
-      <c r="D11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="H11" t="s">
+      <c r="D13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="H13" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>